<commit_message>
prueba de los nuevos modulos sin terminar la visualizacion de los inmuebles
</commit_message>
<xml_diff>
--- a/Excel/Reporte.xlsx
+++ b/Excel/Reporte.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\Proyecto\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{09695E0C-427F-4E60-BCBB-3246E72AEF48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A6FA4DD-29C2-43B5-849B-CA9B58013EB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{D9153E57-445E-4CBB-85F5-0C293230246B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Ventas Habitacionales</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Oficina</t>
   </si>
   <si>
-    <t>Lugar</t>
-  </si>
-  <si>
-    <t>Col./Fracc.</t>
-  </si>
-  <si>
     <t>Domicilio</t>
   </si>
   <si>
@@ -74,26 +68,20 @@
     <t>Asesor</t>
   </si>
   <si>
-    <t>Observaciones</t>
-  </si>
-  <si>
-    <t>Ubicación en el mapa</t>
-  </si>
-  <si>
-    <t>Fotografías</t>
-  </si>
-  <si>
-    <t>Recorrido Virtual</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Colonia</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -109,6 +97,18 @@
     <font>
       <sz val="24"/>
       <color theme="0"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Montserrat"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Montserrat"/>
     </font>
   </fonts>
@@ -145,12 +145,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -473,31 +473,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FF35795-8658-4B0B-A24B-F152BD9967EC}">
-  <dimension ref="A1:P8"/>
+  <dimension ref="A1:Q8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" style="1"/>
-    <col min="2" max="4" width="15.77734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="40.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="30.77734375" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.5546875" style="1"/>
-    <col min="9" max="9" width="50.77734375" style="1" customWidth="1"/>
-    <col min="10" max="11" width="11.5546875" style="1"/>
-    <col min="12" max="12" width="50.77734375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="24.33203125" style="1" customWidth="1"/>
-    <col min="14" max="14" width="13.109375" style="1" customWidth="1"/>
-    <col min="15" max="15" width="23.109375" style="1" customWidth="1"/>
-    <col min="16" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="10.77734375" style="4" customWidth="1"/>
+    <col min="2" max="3" width="20.77734375" style="4" customWidth="1"/>
+    <col min="4" max="5" width="50.77734375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="30.77734375" style="4" customWidth="1"/>
+    <col min="7" max="8" width="25.77734375" style="4" customWidth="1"/>
+    <col min="9" max="10" width="50.77734375" style="4" customWidth="1"/>
+    <col min="11" max="11" width="25.77734375" style="4" customWidth="1"/>
+    <col min="12" max="12" width="11.5546875" style="1"/>
+    <col min="13" max="13" width="50.77734375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="13.109375" style="1" customWidth="1"/>
+    <col min="16" max="16" width="23.109375" style="1" customWidth="1"/>
+    <col min="17" max="16384" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -511,13 +512,14 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
       <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="5"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -529,70 +531,61 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:16" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="19.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="G5" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="J5" s="4" t="s">
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="8" spans="1:17" ht="60" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F8" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="N5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I6" s="3"/>
-    </row>
-    <row r="8" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:O4"/>
+    <mergeCell ref="A3:K4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>